<commit_message>
add column in passenger table
</commit_message>
<xml_diff>
--- a/database/dbexcel.xlsx
+++ b/database/dbexcel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="회원가입" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="295">
   <si>
     <t>member(회원)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1108,35 +1108,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>default W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar2(200)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 승인 대기 중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seq_approve_driver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ad_detail 승인설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ci_max_people</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_regdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sysdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_people_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Y: 승인 W:대기 C:취소</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>default W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar2(200)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default 승인 대기 중</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seq_approve_driver</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ad_detail 승인설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ci_max_people</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c_regdate</t>
+    <t>is_approve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 'W'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운전자가 승인 한 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply_date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1144,15 +1180,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sysdate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c_people_count</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default 1</t>
+    <t>default sysdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탑승신청 일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_deletion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 'N'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탑승자 삭제여부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1730,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2292,7 +2340,7 @@
     </row>
     <row r="27" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>19</v>
@@ -2412,13 +2460,13 @@
     </row>
     <row r="35" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="15" t="s">
         <v>279</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>280</v>
       </c>
       <c r="E35" s="7">
         <v>2</v>
@@ -2435,13 +2483,13 @@
     </row>
     <row r="36" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -2616,10 +2664,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2687,48 +2735,90 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B13" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D13" s="33">
         <v>0.31597222222222221</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E13" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2740,7 +2830,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A33" sqref="A33:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3268,7 +3358,7 @@
         <v>24</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
@@ -3354,10 +3444,10 @@
         <v>270</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D37" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="F37" s="7">
         <v>2</v>
@@ -3374,13 +3464,13 @@
     </row>
     <row r="38" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B38" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>273</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>